<commit_message>
Cambios diccionario de datos
</commit_message>
<xml_diff>
--- a/Diagramas/Diccionario de datos ptc.xlsx
+++ b/Diagramas/Diccionario de datos ptc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\IdeaProjects\Expo-2024-Habit\Diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3D2DF3-D2F7-4C92-8206-CE18AC991C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A6B4A1-F1BD-48B8-9451-08BA9C0D1609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="181">
   <si>
     <t>tb_clientes</t>
   </si>
@@ -576,6 +576,9 @@
   </si>
   <si>
     <t>Identificador del Administrador asociado al blog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campo para almacenar la fecha de inscripción del blog </t>
   </si>
 </sst>
 </file>
@@ -879,6 +882,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -890,12 +899,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1231,7 +1234,7 @@
   <dimension ref="B2:CO117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1247,14 +1250,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="23" t="s">
@@ -1425,14 +1428,14 @@
       <c r="G10"/>
     </row>
     <row r="11" spans="2:12" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1596,14 +1599,14 @@
       <c r="G19"/>
     </row>
     <row r="20" spans="2:11" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="22" t="s">
@@ -1681,14 +1684,14 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="2:11" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="21" t="s">
@@ -1762,14 +1765,14 @@
       <c r="G29"/>
     </row>
     <row r="30" spans="2:11" ht="17.399999999999999">
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" s="23" t="s">
@@ -2072,14 +2075,14 @@
       <c r="G45" s="40"/>
     </row>
     <row r="46" spans="2:11" ht="17.399999999999999">
-      <c r="B46" s="55" t="s">
+      <c r="B46" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
     </row>
     <row r="47" spans="2:11">
       <c r="B47" s="21" t="s">
@@ -2214,14 +2217,14 @@
       <c r="K53" s="6"/>
     </row>
     <row r="54" spans="2:11" ht="17.399999999999999">
-      <c r="B54" s="55" t="s">
+      <c r="B54" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="55"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="57"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
@@ -2313,14 +2316,14 @@
       <c r="G59"/>
     </row>
     <row r="60" spans="2:11" ht="17.399999999999999">
-      <c r="B60" s="55" t="s">
+      <c r="B60" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="55"/>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="55"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="57"/>
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="21" t="s">
@@ -2404,14 +2407,14 @@
       <c r="G65"/>
     </row>
     <row r="66" spans="2:93" ht="17.399999999999999">
-      <c r="B66" s="55" t="s">
+      <c r="B66" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C66" s="55"/>
-      <c r="D66" s="55"/>
-      <c r="E66" s="55"/>
-      <c r="F66" s="55"/>
-      <c r="G66" s="55"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="57"/>
     </row>
     <row r="67" spans="2:93">
       <c r="B67" s="21" t="s">
@@ -2627,14 +2630,14 @@
       <c r="D74" s="3"/>
     </row>
     <row r="75" spans="2:93" ht="17.399999999999999">
-      <c r="B75" s="55" t="s">
+      <c r="B75" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="C75" s="55"/>
-      <c r="D75" s="55"/>
-      <c r="E75" s="55"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="55"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="57"/>
+      <c r="F75" s="57"/>
+      <c r="G75" s="57"/>
     </row>
     <row r="76" spans="2:93">
       <c r="B76" s="21" t="s">
@@ -2718,14 +2721,14 @@
       <c r="G80"/>
     </row>
     <row r="81" spans="2:7" ht="17.399999999999999">
-      <c r="B81" s="52" t="s">
+      <c r="B81" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="C81" s="53"/>
-      <c r="D81" s="53"/>
-      <c r="E81" s="53"/>
-      <c r="F81" s="53"/>
-      <c r="G81" s="54"/>
+      <c r="C81" s="55"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="56"/>
     </row>
     <row r="82" spans="2:7">
       <c r="B82" s="21" t="s">
@@ -2855,14 +2858,14 @@
       <c r="G89"/>
     </row>
     <row r="90" spans="2:7" ht="17.399999999999999">
-      <c r="B90" s="52" t="s">
+      <c r="B90" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="C90" s="53"/>
-      <c r="D90" s="53"/>
-      <c r="E90" s="53"/>
-      <c r="F90" s="53"/>
-      <c r="G90" s="54"/>
+      <c r="C90" s="55"/>
+      <c r="D90" s="55"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="55"/>
+      <c r="G90" s="56"/>
     </row>
     <row r="91" spans="2:7">
       <c r="B91" s="21" t="s">
@@ -2962,14 +2965,14 @@
       <c r="G96"/>
     </row>
     <row r="97" spans="2:7" ht="17.399999999999999">
-      <c r="B97" s="52" t="s">
+      <c r="B97" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="C97" s="53"/>
-      <c r="D97" s="53"/>
-      <c r="E97" s="53"/>
-      <c r="F97" s="53"/>
-      <c r="G97" s="54"/>
+      <c r="C97" s="55"/>
+      <c r="D97" s="55"/>
+      <c r="E97" s="55"/>
+      <c r="F97" s="55"/>
+      <c r="G97" s="56"/>
     </row>
     <row r="98" spans="2:7">
       <c r="B98" s="21" t="s">
@@ -3046,14 +3049,14 @@
       </c>
     </row>
     <row r="103" spans="2:7" ht="17.399999999999999">
-      <c r="B103" s="52" t="s">
+      <c r="B103" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="C103" s="53"/>
-      <c r="D103" s="53"/>
-      <c r="E103" s="53"/>
-      <c r="F103" s="53"/>
-      <c r="G103" s="54"/>
+      <c r="C103" s="55"/>
+      <c r="D103" s="55"/>
+      <c r="E103" s="55"/>
+      <c r="F103" s="55"/>
+      <c r="G103" s="56"/>
     </row>
     <row r="104" spans="2:7">
       <c r="B104" s="21" t="s">
@@ -3146,14 +3149,14 @@
       </c>
     </row>
     <row r="110" spans="2:7" ht="17.399999999999999">
-      <c r="B110" s="52" t="s">
+      <c r="B110" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="C110" s="53"/>
-      <c r="D110" s="53"/>
-      <c r="E110" s="53"/>
-      <c r="F110" s="53"/>
-      <c r="G110" s="54"/>
+      <c r="C110" s="55"/>
+      <c r="D110" s="55"/>
+      <c r="E110" s="55"/>
+      <c r="F110" s="55"/>
+      <c r="G110" s="56"/>
     </row>
     <row r="111" spans="2:7">
       <c r="B111" s="21" t="s">
@@ -3240,24 +3243,24 @@
         <v>176</v>
       </c>
       <c r="G115" s="47" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
     </row>
     <row r="116" spans="2:7">
       <c r="B116" s="31"/>
-      <c r="C116" s="56" t="s">
+      <c r="C116" s="52" t="s">
         <v>177</v>
       </c>
       <c r="D116" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E116" s="57" t="s">
+      <c r="E116" s="53" t="s">
         <v>58</v>
       </c>
       <c r="F116" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G116" s="56" t="s">
+      <c r="G116" s="52" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3273,7 +3276,7 @@
       </c>
       <c r="E117" s="48"/>
       <c r="F117" s="46" t="s">
-        <v>167</v>
+        <v>84</v>
       </c>
       <c r="G117" s="47" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
Diccionario de datos uwu
</commit_message>
<xml_diff>
--- a/Diagramas/Diccionario de datos ptc.xlsx
+++ b/Diagramas/Diccionario de datos ptc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\IdeaProjects\Expo-2024-Habit\Diagramas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\OneDrive\Desktop\2024\Expo-2024-Habit\Diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A6B4A1-F1BD-48B8-9451-08BA9C0D1609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED19344-0B00-4F4E-B961-3FD457F0FD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="182">
   <si>
     <t>tb_clientes</t>
   </si>
@@ -579,13 +579,16 @@
   </si>
   <si>
     <t xml:space="preserve">Campo para almacenar la fecha de inscripción del blog </t>
+  </si>
+  <si>
+    <t>Identificador de la zona preferida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,6 +651,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -681,7 +693,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -713,43 +725,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -757,7 +732,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -888,16 +863,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1231,33 +1200,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:CO117"/>
+  <dimension ref="B2:CO119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G115" sqref="G115"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77:G77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="20.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="33.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="52.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="52.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="2:12" s="5" customFormat="1" ht="17.25">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="23" t="s">
@@ -1427,15 +1396,15 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="2:12" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B11" s="57" t="s">
+    <row r="11" spans="2:12" s="5" customFormat="1" ht="17.25">
+      <c r="B11" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1598,15 +1567,15 @@
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="2:11" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B20" s="57" t="s">
+    <row r="20" spans="2:11" s="5" customFormat="1" ht="17.25">
+      <c r="B20" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="22" t="s">
@@ -1683,15 +1652,15 @@
       <c r="F24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="2:11" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="B25" s="57" t="s">
+    <row r="25" spans="2:11" s="5" customFormat="1" ht="17.25">
+      <c r="B25" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="21" t="s">
@@ -1764,15 +1733,15 @@
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="2:11" ht="17.399999999999999">
-      <c r="B30" s="57" t="s">
+    <row r="30" spans="2:11" ht="17.25">
+      <c r="B30" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" s="23" t="s">
@@ -2074,15 +2043,15 @@
       <c r="F45" s="41"/>
       <c r="G45" s="40"/>
     </row>
-    <row r="46" spans="2:11" ht="17.399999999999999">
-      <c r="B46" s="57" t="s">
+    <row r="46" spans="2:11" ht="17.25">
+      <c r="B46" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
     </row>
     <row r="47" spans="2:11">
       <c r="B47" s="21" t="s">
@@ -2216,15 +2185,15 @@
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
     </row>
-    <row r="54" spans="2:11" ht="17.399999999999999">
-      <c r="B54" s="57" t="s">
+    <row r="54" spans="2:11" ht="17.25">
+      <c r="B54" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
@@ -2315,15 +2284,15 @@
       <c r="F59"/>
       <c r="G59"/>
     </row>
-    <row r="60" spans="2:11" ht="17.399999999999999">
-      <c r="B60" s="57" t="s">
+    <row r="60" spans="2:11" ht="17.25">
+      <c r="B60" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="54"/>
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="21" t="s">
@@ -2406,15 +2375,15 @@
       <c r="F65"/>
       <c r="G65"/>
     </row>
-    <row r="66" spans="2:93" ht="17.399999999999999">
-      <c r="B66" s="57" t="s">
+    <row r="66" spans="2:93" ht="17.25">
+      <c r="B66" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="C66" s="57"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="57"/>
-      <c r="F66" s="57"/>
-      <c r="G66" s="57"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="54"/>
+      <c r="F66" s="54"/>
+      <c r="G66" s="54"/>
     </row>
     <row r="67" spans="2:93">
       <c r="B67" s="21" t="s">
@@ -2627,674 +2596,692 @@
       </c>
     </row>
     <row r="74" spans="2:93">
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="2:93" ht="17.399999999999999">
-      <c r="B75" s="57" t="s">
+      <c r="B74" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="39"/>
+      <c r="F74" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G74" s="37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="2:93">
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="2:93" ht="17.25">
+      <c r="B77" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="C75" s="57"/>
-      <c r="D75" s="57"/>
-      <c r="E75" s="57"/>
-      <c r="F75" s="57"/>
-      <c r="G75" s="57"/>
-    </row>
-    <row r="76" spans="2:93">
-      <c r="B76" s="21" t="s">
+      <c r="C77" s="55"/>
+      <c r="D77" s="55"/>
+      <c r="E77" s="55"/>
+      <c r="F77" s="55"/>
+      <c r="G77" s="55"/>
+    </row>
+    <row r="78" spans="2:93">
+      <c r="B78" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C78" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D76" s="21" t="s">
+      <c r="D78" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E76" s="22" t="s">
+      <c r="E78" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F76" s="21" t="s">
+      <c r="F78" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="21" t="s">
+      <c r="G78" s="21" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="2:93">
-      <c r="B77" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D77" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="13"/>
-      <c r="F77" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G77" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="2:93">
-      <c r="B78" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D78" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="27"/>
-      <c r="F78" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G78" s="26" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="79" spans="2:93">
       <c r="B79" s="31" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D79" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="2:93" ht="15" customHeight="1">
+      <c r="B80" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="27"/>
+      <c r="F80" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="G79" s="11" t="s">
+      <c r="G80" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="13"/>
+      <c r="F81" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G81" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="2:93" ht="15" customHeight="1">
-      <c r="C80" s="2"/>
-      <c r="D80"/>
-      <c r="E80" s="1"/>
-      <c r="F80"/>
-      <c r="G80"/>
-    </row>
-    <row r="81" spans="2:7" ht="17.399999999999999">
-      <c r="B81" s="54" t="s">
+    <row r="82" spans="2:7">
+      <c r="C82" s="2"/>
+      <c r="D82"/>
+      <c r="E82" s="1"/>
+      <c r="F82"/>
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="2:7" ht="17.25">
+      <c r="B83" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="C81" s="55"/>
-      <c r="D81" s="55"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55"/>
-      <c r="G81" s="56"/>
-    </row>
-    <row r="82" spans="2:7">
-      <c r="B82" s="21" t="s">
+      <c r="C83" s="54"/>
+      <c r="D83" s="54"/>
+      <c r="E83" s="54"/>
+      <c r="F83" s="54"/>
+      <c r="G83" s="54"/>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="C84" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D82" s="21" t="s">
+      <c r="D84" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E82" s="22" t="s">
+      <c r="E84" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F82" s="21" t="s">
+      <c r="F84" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G82" s="21" t="s">
+      <c r="G84" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="2:7">
-      <c r="B83" s="31" t="s">
+    <row r="85" spans="2:7">
+      <c r="B85" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C85" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D83" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="13"/>
-      <c r="F83" s="12" t="s">
+      <c r="D85" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="13"/>
+      <c r="F85" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G83" s="11" t="s">
+      <c r="G85" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="84" spans="2:7">
-      <c r="B84" s="28" t="s">
+    <row r="86" spans="2:7">
+      <c r="B86" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="C84" s="26" t="s">
+      <c r="C86" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="D84" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="27"/>
-      <c r="F84" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G84" s="26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7">
-      <c r="B85" s="37"/>
-      <c r="C85" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="D85" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E85" s="39"/>
-      <c r="F85" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="G85" s="37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7">
-      <c r="B86" s="26"/>
-      <c r="C86" s="26" t="s">
-        <v>139</v>
-      </c>
       <c r="D86" s="28" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="E86" s="27"/>
       <c r="F86" s="28" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="G86" s="26" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="2:7">
       <c r="B87" s="37"/>
       <c r="C87" s="37" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D87" s="38" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="E87" s="39"/>
       <c r="F87" s="38" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G87" s="37" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="2:7">
       <c r="B88" s="26"/>
       <c r="C88" s="26" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="E88" s="27"/>
       <c r="F88" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G88" s="26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89" s="37"/>
+      <c r="C89" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D89" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E89" s="39"/>
+      <c r="F89" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="G89" s="37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7">
+      <c r="B90" s="26"/>
+      <c r="C90" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D90" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E90" s="27"/>
+      <c r="F90" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G88" s="26" t="s">
+      <c r="G90" s="26" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="2:7">
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89" s="1"/>
-      <c r="F89"/>
-      <c r="G89"/>
-    </row>
-    <row r="90" spans="2:7" ht="17.399999999999999">
-      <c r="B90" s="54" t="s">
+    <row r="91" spans="2:7">
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91" s="1"/>
+      <c r="F91"/>
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="2:7" ht="17.25">
+      <c r="B92" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="C90" s="55"/>
-      <c r="D90" s="55"/>
-      <c r="E90" s="55"/>
-      <c r="F90" s="55"/>
-      <c r="G90" s="56"/>
-    </row>
-    <row r="91" spans="2:7">
-      <c r="B91" s="21" t="s">
+      <c r="C92" s="54"/>
+      <c r="D92" s="54"/>
+      <c r="E92" s="54"/>
+      <c r="F92" s="54"/>
+      <c r="G92" s="54"/>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="21" t="s">
+      <c r="C93" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D91" s="21" t="s">
+      <c r="D93" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E91" s="22" t="s">
+      <c r="E93" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F91" s="21" t="s">
+      <c r="F93" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G91" s="21" t="s">
+      <c r="G93" s="21" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7">
-      <c r="B92" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="13"/>
-      <c r="F92" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G92" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7">
-      <c r="B93" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C93" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D93" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="27"/>
-      <c r="F93" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G93" s="36" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="94" spans="2:7">
       <c r="B94" s="31" t="s">
-        <v>135</v>
+        <v>7</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="D94" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E94" s="13"/>
       <c r="F94" s="12" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="G94" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="2:7">
-      <c r="B95" s="28"/>
+      <c r="B95" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="C95" s="36" t="s">
-        <v>152</v>
+        <v>8</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="E95" s="27"/>
       <c r="F95" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="G95" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7">
+      <c r="B96" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="13"/>
+      <c r="F96" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G96" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" s="28"/>
+      <c r="C97" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D97" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E97" s="27"/>
+      <c r="F97" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="G95" s="36" t="s">
+      <c r="G97" s="36" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="2:7">
-      <c r="C96"/>
-      <c r="D96"/>
-      <c r="E96" s="1"/>
-      <c r="F96"/>
-      <c r="G96"/>
-    </row>
-    <row r="97" spans="2:7" ht="17.399999999999999">
-      <c r="B97" s="54" t="s">
+    <row r="98" spans="2:7">
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="E98" s="1"/>
+      <c r="F98"/>
+      <c r="G98"/>
+    </row>
+    <row r="99" spans="2:7" ht="17.25">
+      <c r="B99" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="C97" s="55"/>
-      <c r="D97" s="55"/>
-      <c r="E97" s="55"/>
-      <c r="F97" s="55"/>
-      <c r="G97" s="56"/>
-    </row>
-    <row r="98" spans="2:7">
-      <c r="B98" s="21" t="s">
+      <c r="C99" s="54"/>
+      <c r="D99" s="54"/>
+      <c r="E99" s="54"/>
+      <c r="F99" s="54"/>
+      <c r="G99" s="54"/>
+    </row>
+    <row r="100" spans="2:7">
+      <c r="B100" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C98" s="21" t="s">
+      <c r="C100" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D98" s="21" t="s">
+      <c r="D100" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E98" s="22" t="s">
+      <c r="E100" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F98" s="21" t="s">
+      <c r="F100" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G98" s="21" t="s">
+      <c r="G100" s="21" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7">
-      <c r="B99" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C99" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D99" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="14"/>
-      <c r="F99" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G99" s="20" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7">
-      <c r="B100" s="28"/>
-      <c r="C100" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="D100" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E100" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F100" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G100" s="36" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="101" spans="2:7">
       <c r="B101" s="31" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C101" s="20" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="D101" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E101" s="14"/>
       <c r="F101" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G101" s="20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="B102" s="28"/>
+      <c r="C102" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D102" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F102" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G102" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="14"/>
+      <c r="F103" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G101" s="20" t="s">
+      <c r="G103" s="20" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="2:7" ht="17.399999999999999">
-      <c r="B103" s="54" t="s">
+    <row r="105" spans="2:7" ht="17.25">
+      <c r="B105" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="C103" s="55"/>
-      <c r="D103" s="55"/>
-      <c r="E103" s="55"/>
-      <c r="F103" s="55"/>
-      <c r="G103" s="56"/>
-    </row>
-    <row r="104" spans="2:7">
-      <c r="B104" s="21" t="s">
+      <c r="C105" s="54"/>
+      <c r="D105" s="54"/>
+      <c r="E105" s="54"/>
+      <c r="F105" s="54"/>
+      <c r="G105" s="54"/>
+    </row>
+    <row r="106" spans="2:7">
+      <c r="B106" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C104" s="21" t="s">
+      <c r="C106" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="21" t="s">
+      <c r="D106" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E104" s="22" t="s">
+      <c r="E106" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F104" s="21" t="s">
+      <c r="F106" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G104" s="21" t="s">
+      <c r="G106" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="2:7">
-      <c r="B105" s="31" t="s">
+    <row r="107" spans="2:7">
+      <c r="B107" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C105" s="20" t="s">
+      <c r="C107" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D105" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="14"/>
-      <c r="F105" s="15" t="s">
+      <c r="D107" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="14"/>
+      <c r="F107" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G105" s="20" t="s">
+      <c r="G107" s="20" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="106" spans="2:7">
-      <c r="B106" s="28"/>
-      <c r="C106" s="36" t="s">
+    <row r="108" spans="2:7">
+      <c r="B108" s="28"/>
+      <c r="C108" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="D106" s="28" t="s">
+      <c r="D108" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E106" s="27"/>
-      <c r="F106" s="28" t="s">
+      <c r="E108" s="27"/>
+      <c r="F108" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="G106" s="36" t="s">
+      <c r="G108" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="2:7">
-      <c r="B107" s="49" t="s">
+    <row r="109" spans="2:7">
+      <c r="B109" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C107" s="50" t="s">
+      <c r="C109" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="D107" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="51"/>
-      <c r="F107" s="49" t="s">
+      <c r="D109" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="51"/>
+      <c r="F109" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="G107" s="50" t="s">
+      <c r="G109" s="50" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="108" spans="2:7">
-      <c r="B108" s="46" t="s">
+    <row r="110" spans="2:7">
+      <c r="B110" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C108" s="47" t="s">
+      <c r="C110" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D108" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="48"/>
-      <c r="F108" s="46" t="s">
+      <c r="D110" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="48"/>
+      <c r="F110" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="G108" s="47" t="s">
+      <c r="G110" s="47" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="17.399999999999999">
-      <c r="B110" s="54" t="s">
+    <row r="112" spans="2:7" ht="17.25">
+      <c r="B112" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="C110" s="55"/>
-      <c r="D110" s="55"/>
-      <c r="E110" s="55"/>
-      <c r="F110" s="55"/>
-      <c r="G110" s="56"/>
-    </row>
-    <row r="111" spans="2:7">
-      <c r="B111" s="21" t="s">
+      <c r="C112" s="54"/>
+      <c r="D112" s="54"/>
+      <c r="E112" s="54"/>
+      <c r="F112" s="54"/>
+      <c r="G112" s="54"/>
+    </row>
+    <row r="113" spans="2:7">
+      <c r="B113" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C111" s="21" t="s">
+      <c r="C113" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D111" s="21" t="s">
+      <c r="D113" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E111" s="22" t="s">
+      <c r="E113" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F111" s="21" t="s">
+      <c r="F113" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G111" s="21" t="s">
+      <c r="G113" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="2:7">
-      <c r="B112" s="31" t="s">
+    <row r="114" spans="2:7">
+      <c r="B114" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C112" s="20" t="s">
+      <c r="C114" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="D112" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="14"/>
-      <c r="F112" s="15" t="s">
+      <c r="D114" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="14"/>
+      <c r="F114" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G112" s="20" t="s">
+      <c r="G114" s="20" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="2:7">
-      <c r="B113" s="28"/>
-      <c r="C113" s="36" t="s">
+    <row r="115" spans="2:7">
+      <c r="B115" s="28"/>
+      <c r="C115" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="D113" s="28" t="s">
+      <c r="D115" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E113" s="27" t="s">
+      <c r="E115" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F113" s="28" t="s">
+      <c r="F115" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G113" s="36" t="s">
+      <c r="G115" s="36" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="114" spans="2:7">
-      <c r="B114" s="49"/>
-      <c r="C114" s="50" t="s">
+    <row r="116" spans="2:7">
+      <c r="B116" s="49"/>
+      <c r="C116" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="D114" s="49" t="s">
+      <c r="D116" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="E114" s="51"/>
-      <c r="F114" s="49" t="s">
+      <c r="E116" s="51"/>
+      <c r="F116" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="G114" s="50" t="s">
+      <c r="G116" s="50" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="115" spans="2:7">
-      <c r="B115" s="46"/>
-      <c r="C115" s="47" t="s">
+    <row r="117" spans="2:7">
+      <c r="B117" s="46"/>
+      <c r="C117" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="D115" s="46" t="s">
+      <c r="D117" s="46" t="s">
         <v>175</v>
-      </c>
-      <c r="E115" s="48"/>
-      <c r="F115" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="G115" s="47" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7">
-      <c r="B116" s="31"/>
-      <c r="C116" s="52" t="s">
-        <v>177</v>
-      </c>
-      <c r="D116" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E116" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="F116" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G116" s="52" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7">
-      <c r="B117" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C117" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="D117" s="46" t="s">
-        <v>9</v>
       </c>
       <c r="E117" s="48"/>
       <c r="F117" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="G117" s="47" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="B118" s="31"/>
+      <c r="C118" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="D118" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="F118" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G118" s="52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C119" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="48"/>
+      <c r="F119" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G117" s="47" t="s">
+      <c r="G119" s="47" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B110:G110"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B97:G97"/>
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="B99:G99"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B112:G112"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B90:G90"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B77:G77"/>
     <mergeCell ref="B60:G60"/>
     <mergeCell ref="B66:G66"/>
     <mergeCell ref="B46:G46"/>

</xml_diff>